<commit_message>
null return and car not match condition resolved
</commit_message>
<xml_diff>
--- a/cache/cars.xlsx
+++ b/cache/cars.xlsx
@@ -2510,7 +2510,7 @@
         <v>1000000</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2519,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="K40">
         <v>0</v>

</xml_diff>

<commit_message>
comments added in some files
</commit_message>
<xml_diff>
--- a/cache/cars.xlsx
+++ b/cache/cars.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -419,9 +419,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -3075,7 +3077,7 @@
     </row>
     <row r="51" spans="1:17">
       <c r="A51">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>17</v>

</xml_diff>